<commit_message>
updated the itenerary to allow downloading of an excel file
</commit_message>
<xml_diff>
--- a/CyberDayInformationSystem/Uploads/test2.xlsx
+++ b/CyberDayInformationSystem/Uploads/test2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cloud\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cloud\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7672E550-F0A2-4226-A559-0C3A7F27AFB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302983FA-2989-46E4-AF67-B00088E86E18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C2B95995-18BD-408F-81AF-67C73A88B389}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C2B95995-18BD-408F-81AF-67C73A88B389}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
   <si>
     <t>Time</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Time Formatter</t>
   </si>
   <si>
-    <t>Arrival</t>
-  </si>
-  <si>
     <t>parking lot 1</t>
   </si>
   <si>
@@ -140,6 +137,12 @@
   </si>
   <si>
     <t>D-Hall</t>
+  </si>
+  <si>
+    <t>Coffee Time</t>
+  </si>
+  <si>
+    <t>muh house</t>
   </si>
 </sst>
 </file>
@@ -624,7 +627,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CCB3A3E-5D05-4496-913C-9A61574B8DCF}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -647,15 +650,15 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="str">
         <f>CONCATENATE(" ",Sheet1!F2)</f>
-        <v xml:space="preserve"> 07:30 AM</v>
+        <v xml:space="preserve"> 09:15 AM</v>
       </c>
       <c r="B2" t="str">
         <f>CONCATENATE(" ",Sheet1!B2)</f>
-        <v xml:space="preserve"> Arrival</v>
+        <v xml:space="preserve"> Coffee Time</v>
       </c>
       <c r="C2" t="str">
         <f>CONCATENATE(" ",Sheet1!C2)</f>
-        <v xml:space="preserve"> Parking Lot 1</v>
+        <v xml:space="preserve"> muh house</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -709,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46A325E8-6DA2-4A4C-9E2B-F67A29B97C8B}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -739,17 +742,17 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
-        <v>0.3125</v>
+        <v>0.38541666666666669</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F2" t="str">
         <f>TEXT(A2, "hh:mm AM/PM")</f>
-        <v>07:30 AM</v>
+        <v>09:15 AM</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -757,10 +760,10 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F3" t="str">
         <f>TEXT(A3, "hh:mm AM/PM")</f>
@@ -772,10 +775,10 @@
         <v>0.35416666666666702</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" ref="F4:F5" si="0">TEXT(A4, "hh:mm AM/PM")</f>
@@ -792,10 +795,10 @@
         <v>0.375</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
@@ -807,10 +810,10 @@
         <v>0.39583333333333298</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" ref="F6:F26" si="1">TEXT(A6, "hh:mm AM/PM")</f>
@@ -822,10 +825,10 @@
         <v>0.41666666666666702</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="1"/>
@@ -837,10 +840,10 @@
         <v>0.4375</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="1"/>
@@ -852,10 +855,10 @@
         <v>0.45833333333333298</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="1"/>
@@ -867,10 +870,10 @@
         <v>0.47916666666666702</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="1"/>
@@ -882,10 +885,10 @@
         <v>0.5</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="1"/>
@@ -897,10 +900,10 @@
         <v>0.52083333333333304</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="1"/>
@@ -912,10 +915,10 @@
         <v>0.54166666666666596</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="1"/>
@@ -927,10 +930,10 @@
         <v>0.5625</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="1"/>
@@ -942,10 +945,10 @@
         <v>0.58333333333333304</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="1"/>
@@ -957,10 +960,10 @@
         <v>0.60416666666666596</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="1"/>
@@ -972,10 +975,10 @@
         <v>0.625</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="1"/>
@@ -987,10 +990,10 @@
         <v>0.64583333333333304</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="1"/>
@@ -1002,10 +1005,10 @@
         <v>0.66666666666666596</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="1"/>
@@ -1017,10 +1020,10 @@
         <v>0.6875</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="1"/>
@@ -1032,10 +1035,10 @@
         <v>0.70833333333333304</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="1"/>
@@ -1047,10 +1050,10 @@
         <v>0.72916666666666596</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="1"/>
@@ -1062,10 +1065,10 @@
         <v>0.75</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="1"/>
@@ -1077,10 +1080,10 @@
         <v>0.77083333333333304</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="1"/>
@@ -1092,10 +1095,10 @@
         <v>0.79166666666666596</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="1"/>
@@ -1107,10 +1110,10 @@
         <v>0.8125</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="1"/>

</xml_diff>